<commit_message>
Import ADJ column from excel budget file.
</commit_message>
<xml_diff>
--- a/forecast/test/test_assets/budget_upload_bad_dash.xlsx
+++ b/forecast/test/test_assets/budget_upload_bad_dash.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minarm\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stronal/PycharmProjects/fft/forecast/test/test_assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1ECF4B13-250F-490B-8653-B01962214048}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0705D13E-3C3B-1346-AF8B-2B89277BEB65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25780" windowHeight="13980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Budgets" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Programme</t>
   </si>
@@ -90,6 +90,15 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>ADJ1</t>
+  </si>
+  <si>
+    <t>ADJ2</t>
+  </si>
+  <si>
+    <t>ADJ3</t>
   </si>
 </sst>
 </file>
@@ -936,22 +945,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8203125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="9.17578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="22.64453125" customWidth="1"/>
-    <col min="5" max="5" width="13.3515625" customWidth="1"/>
-    <col min="7" max="7" width="7.17578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="7.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1006,8 +1015,17 @@
       <c r="R1" t="s">
         <v>16</v>
       </c>
+      <c r="S1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>109189</v>
       </c>
@@ -1063,7 +1081,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>888888</v>
       </c>
@@ -1119,7 +1137,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>109189</v>
       </c>
@@ -1393,18 +1411,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1427,14 +1445,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ADF255A-1CA2-4DE5-95FF-3D43C4BC1A95}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F34B647-70B2-425E-B00E-F8374E364F8C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -1449,4 +1459,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ADF255A-1CA2-4DE5-95FF-3D43C4BC1A95}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
LST 1469 upload budgets from adjustment columns
* Requested by Finance: the adjustment column contains changes to budgets related to past months.

* Changed python version to 3.9.5.
</commit_message>
<xml_diff>
--- a/forecast/test/test_assets/budget_upload_bad_dash.xlsx
+++ b/forecast/test/test_assets/budget_upload_bad_dash.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minarm\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stronal/PycharmProjects/fft/forecast/test/test_assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1ECF4B13-250F-490B-8653-B01962214048}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0705D13E-3C3B-1346-AF8B-2B89277BEB65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25780" windowHeight="13980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Budgets" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Programme</t>
   </si>
@@ -90,6 +90,15 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>ADJ1</t>
+  </si>
+  <si>
+    <t>ADJ2</t>
+  </si>
+  <si>
+    <t>ADJ3</t>
   </si>
 </sst>
 </file>
@@ -936,22 +945,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8203125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="9.17578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="22.64453125" customWidth="1"/>
-    <col min="5" max="5" width="13.3515625" customWidth="1"/>
-    <col min="7" max="7" width="7.17578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="7.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1006,8 +1015,17 @@
       <c r="R1" t="s">
         <v>16</v>
       </c>
+      <c r="S1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>109189</v>
       </c>
@@ -1063,7 +1081,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>888888</v>
       </c>
@@ -1119,7 +1137,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>109189</v>
       </c>
@@ -1393,18 +1411,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1427,14 +1445,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ADF255A-1CA2-4DE5-95FF-3D43C4BC1A95}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F34B647-70B2-425E-B00E-F8374E364F8C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -1449,4 +1459,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ADF255A-1CA2-4DE5-95FF-3D43C4BC1A95}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>